<commit_message>
removed "error" in excel
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Addition" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>#</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -576,13 +576,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -593,13 +593,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -712,13 +712,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -763,13 +763,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -780,13 +780,13 @@
         <v>0</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -797,13 +797,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -871,13 +871,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -888,13 +888,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -945,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -956,13 +956,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1056,13 +1056,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1073,13 +1073,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1181,7 +1181,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1192,13 +1192,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>